<commit_message>
25/2/16 correlation and normals
</commit_message>
<xml_diff>
--- a/Data/EXO/DESeq/Pc3EXOCavin2.xlsx
+++ b/Data/EXO/DESeq/Pc3EXOCavin2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Pc3EXOCavin2" sheetId="1" r:id="rId1"/>
@@ -1461,7 +1461,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1576,6 +1576,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1621,11 +1630,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1950,7 +1960,7 @@
   <dimension ref="A1:G365"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,26 +2885,26 @@
         <v>8.3072239089421199E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="4">
         <v>273.686672047721</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="4">
         <v>1.1620689521474901</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="4">
         <v>0.45566715259777901</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="4">
         <v>2.5502583311579099</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="4">
         <v>1.07643124412571E-2</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="4">
         <v>9.6609704160282306E-2</v>
       </c>
     </row>

</xml_diff>